<commit_message>
Updated a parts list
</commit_message>
<xml_diff>
--- a/Schematics/BOM/Main.xlsx
+++ b/Schematics/BOM/Main.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,12 +10,20 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DF345F65-2549-49D4-B4F4-361C1B0FD438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -367,7 +375,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1215,19 +1223,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1261,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1293,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1313,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
@@ -1333,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1353,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1376,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1408,7 +1416,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1440,7 +1448,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1472,7 +1480,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1504,7 +1512,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1536,7 +1544,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1568,7 +1576,7 @@
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1600,7 +1608,7 @@
       </c>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1632,7 +1640,7 @@
       </c>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1664,7 +1672,7 @@
       </c>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1696,7 +1704,7 @@
       </c>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1728,7 +1736,7 @@
       </c>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1760,7 +1768,7 @@
       </c>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1792,7 +1800,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1815,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1841,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1864,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1887,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1910,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1933,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1956,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1979,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2005,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2028,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2051,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2074,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2097,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2174,6 +2182,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E0320BEE2E6FA4F8CC2F7CE39313111" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4f74ee6864528a11bd38506408ce6cf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cbbf7a48-3d9d-4319-ac59-4b980b275aab" xmlns:ns4="1508e5c0-558d-461e-8c70-700d0e894f7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="db6615b31d6e1ba496bdf5af2269d99c" ns3:_="" ns4:_="">
     <xsd:import namespace="cbbf7a48-3d9d-4319-ac59-4b980b275aab"/>
@@ -2382,36 +2405,11 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584D6917-1633-4ABF-AEE2-D02B7EB20D2F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB498C7-35A6-4366-9E40-4723A4B5CA66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cbbf7a48-3d9d-4319-ac59-4b980b275aab"/>
-    <ds:schemaRef ds:uri="1508e5c0-558d-461e-8c70-700d0e894f7a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2425,18 +2423,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB498C7-35A6-4366-9E40-4723A4B5CA66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584D6917-1633-4ABF-AEE2-D02B7EB20D2F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="cbbf7a48-3d9d-4319-ac59-4b980b275aab"/>
     <ds:schemaRef ds:uri="1508e5c0-558d-461e-8c70-700d0e894f7a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cbbf7a48-3d9d-4319-ac59-4b980b275aab"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>